<commit_message>
fixed typo in 468 old crypto fastq filename .tz rather than .gz
</commit_message>
<xml_diff>
--- a/old_database/crypto/fastqFiles/fastq_468.xlsx
+++ b/old_database/crypto/fastqFiles/fastq_468.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">sequence/run_468_samples/fastq_reformat/s_4_withindex_sequence_1206_37.fastq.gz</t>
   </si>
   <si>
-    <t xml:space="preserve">sequence/run_468_samples/fastq_reformat/s_4_withindex_sequence_1207_30.fastq.tz</t>
+    <t xml:space="preserve">sequence/run_468_samples/fastq_reformat/s_4_withindex_sequence_1207_30.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">sequence/run_468_samples/fastq_reformat/s_4_withindex_sequence_1207_37.fastq.gz</t>
@@ -202,7 +202,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>